<commit_message>
Updated Burndown Chart + Scrum + 1 wireframe
</commit_message>
<xml_diff>
--- a/Project Management/Scrum/Burndown chart.xlsx
+++ b/Project Management/Scrum/Burndown chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8dbff66645a1af34/Documenten/Periode9-ExamenOefening/Project Management/Scrum/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackv\Documents\2 School Programming\Periode9-ExamenOefening\Project Management\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{A692E1F0-5FB1-4ADC-A3B3-E6CBC109E6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D3CC83F-C3C8-4DA9-9C75-A747CA94DFB6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3435B2C-9895-4F8A-B7BB-0DF8B1532924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D64FC014-072E-4862-83BE-4A77B874CE33}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D64FC014-072E-4862-83BE-4A77B874CE33}"/>
   </bookViews>
   <sheets>
     <sheet name="BurndownChart" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
   <si>
     <t>Taak</t>
   </si>
@@ -496,7 +496,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -670,10 +670,10 @@
                   <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1607,10 +1607,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1930,19 +1926,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8170B0-2E68-477D-80A9-FF8E7DC32F40}">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -1960,7 +1956,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1980,7 +1976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>24</v>
       </c>
@@ -1994,7 +1990,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>23</v>
       </c>
@@ -2008,7 +2004,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -2022,7 +2018,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>26</v>
       </c>
@@ -2038,7 +2034,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>25</v>
       </c>
@@ -2052,7 +2048,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>14</v>
       </c>
@@ -2062,7 +2058,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>28</v>
       </c>
@@ -2076,7 +2072,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>27</v>
       </c>
@@ -2090,7 +2086,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>30</v>
       </c>
@@ -2104,7 +2100,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>31</v>
       </c>
@@ -2118,7 +2114,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>42</v>
       </c>
@@ -2132,7 +2128,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>32</v>
       </c>
@@ -2146,7 +2142,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>29</v>
       </c>
@@ -2163,7 +2159,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>15</v>
       </c>
@@ -2173,7 +2169,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>33</v>
       </c>
@@ -2187,7 +2183,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>35</v>
       </c>
@@ -2201,7 +2197,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>43</v>
       </c>
@@ -2215,7 +2211,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>58</v>
       </c>
@@ -2229,7 +2225,7 @@
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>34</v>
       </c>
@@ -2243,7 +2239,7 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>16</v>
       </c>
@@ -2253,7 +2249,7 @@
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>41</v>
       </c>
@@ -2267,7 +2263,7 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>40</v>
       </c>
@@ -2281,7 +2277,7 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>36</v>
       </c>
@@ -2290,12 +2286,12 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2" t="s">
-        <v>73</v>
+      <c r="E25" s="2">
+        <v>4</v>
       </c>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>39</v>
       </c>
@@ -2309,7 +2305,7 @@
       </c>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>38</v>
       </c>
@@ -2318,12 +2314,12 @@
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2" t="s">
-        <v>73</v>
+      <c r="E27" s="2">
+        <v>3</v>
       </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>62</v>
       </c>
@@ -2333,7 +2329,7 @@
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>37</v>
       </c>
@@ -2342,12 +2338,12 @@
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="2" t="s">
-        <v>73</v>
+      <c r="E29" s="2">
+        <v>1</v>
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>44</v>
       </c>
@@ -2356,12 +2352,12 @@
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="2" t="s">
-        <v>73</v>
+      <c r="E30" s="2">
+        <v>1</v>
       </c>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>59</v>
       </c>
@@ -2370,14 +2366,14 @@
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="2" t="s">
-        <v>73</v>
+      <c r="E31" s="2">
+        <v>3</v>
       </c>
       <c r="F31" s="2"/>
       <c r="I31" s="20"/>
       <c r="K31" s="21"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>60</v>
       </c>
@@ -2386,14 +2382,14 @@
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="2" t="s">
-        <v>73</v>
+      <c r="E32" s="2">
+        <v>3</v>
       </c>
       <c r="F32" s="2"/>
       <c r="I32" s="20"/>
       <c r="K32" s="21"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>61</v>
       </c>
@@ -2409,7 +2405,7 @@
       <c r="I33" s="20"/>
       <c r="K33" s="21"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>63</v>
       </c>
@@ -2421,7 +2417,7 @@
       <c r="I34" s="20"/>
       <c r="K34" s="21"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>64</v>
       </c>
@@ -2437,7 +2433,7 @@
       <c r="I35" s="20"/>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>65</v>
       </c>
@@ -2451,7 +2447,7 @@
       </c>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>66</v>
       </c>
@@ -2465,7 +2461,7 @@
       </c>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>17</v>
       </c>
@@ -2475,7 +2471,7 @@
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>67</v>
       </c>
@@ -2489,7 +2485,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>68</v>
       </c>
@@ -2503,7 +2499,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>69</v>
       </c>
@@ -2517,7 +2513,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>70</v>
       </c>
@@ -2531,7 +2527,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>18</v>
       </c>
@@ -2541,7 +2537,7 @@
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>71</v>
       </c>
@@ -2555,7 +2551,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>19</v>
       </c>
@@ -2565,7 +2561,7 @@
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>45</v>
       </c>
@@ -2579,7 +2575,7 @@
       </c>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>46</v>
       </c>
@@ -2593,7 +2589,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>47</v>
       </c>
@@ -2607,7 +2603,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>20</v>
       </c>
@@ -2617,7 +2613,7 @@
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>48</v>
       </c>
@@ -2631,7 +2627,7 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>49</v>
       </c>
@@ -2645,7 +2641,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>50</v>
       </c>
@@ -2659,7 +2655,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>72</v>
       </c>
@@ -2669,7 +2665,7 @@
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>52</v>
       </c>
@@ -2683,7 +2679,7 @@
       </c>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>51</v>
       </c>
@@ -2697,7 +2693,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>53</v>
       </c>
@@ -2711,7 +2707,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>21</v>
       </c>
@@ -2721,7 +2717,7 @@
       <c r="E57" s="13"/>
       <c r="F57" s="13"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>54</v>
       </c>
@@ -2735,7 +2731,7 @@
       </c>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>22</v>
       </c>
@@ -2745,7 +2741,7 @@
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>57</v>
       </c>
@@ -2759,7 +2755,7 @@
       </c>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>56</v>
       </c>
@@ -2773,7 +2769,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>55</v>
       </c>
@@ -2787,7 +2783,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
         <v>74</v>
       </c>
@@ -2797,7 +2793,7 @@
       <c r="E63" s="13"/>
       <c r="F63" s="13"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>75</v>
       </c>
@@ -2811,7 +2807,7 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>76</v>
       </c>
@@ -2825,7 +2821,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
         <v>77</v>
       </c>
@@ -2839,7 +2835,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="14" t="s">
         <v>4</v>
       </c>
@@ -2857,14 +2853,14 @@
       </c>
       <c r="E67" s="16">
         <f>D$67-SUM(E3:E62)</f>
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F67" s="16">
         <f>E$67-SUM(F3:F62)</f>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="17" t="s">
         <v>2</v>
       </c>

</xml_diff>